<commit_message>
Ui: default export template variables fix
</commit_message>
<xml_diff>
--- a/TransferLogger.Ui/Resources/Excel/ExportTemplate.xlsx
+++ b/TransferLogger.Ui/Resources/Excel/ExportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TransferLogger\TransferLogger.Ui\Resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6D33E8-D317-4E3B-BCB8-E05517978820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5353F92-13B8-4579-A658-C3E724BF1336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3030" yWindow="1830" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>APPLICANT NAME:</t>
   </si>
@@ -92,9 +92,6 @@
     <t>SUGGESTED</t>
   </si>
   <si>
-    <t>Application ID</t>
-  </si>
-  <si>
     <t>%AppId%</t>
   </si>
   <si>
@@ -120,6 +117,15 @@
   </si>
   <si>
     <t>%SuggestedCourse%</t>
+  </si>
+  <si>
+    <t>%Transfer%</t>
+  </si>
+  <si>
+    <t>%Comment%</t>
+  </si>
+  <si>
+    <t>APPLICATION ID:</t>
   </si>
 </sst>
 </file>
@@ -148,7 +154,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,12 +173,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -216,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -224,7 +224,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +507,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,10 +523,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -538,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -546,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -556,7 +555,7 @@
     <row r="6" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -578,23 +577,27 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>